<commit_message>
More tests on the new aircraft models.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/AGILE-NTP/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/AGILE-NTP/WEIGHTS/Weights.xlsx
@@ -308,7 +308,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>1200.0</v>
+        <v>1100.0</v>
       </c>
     </row>
     <row r="3">
@@ -346,7 +346,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>48010.150825739336</v>
+        <v>33735.068110578824</v>
       </c>
     </row>
     <row r="7">
@@ -357,7 +357,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>48010.150825739336</v>
+        <v>33735.068110578824</v>
       </c>
     </row>
     <row r="8">
@@ -368,7 +368,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>46569.846300967154</v>
+        <v>32723.01606726146</v>
       </c>
     </row>
     <row r="9">
@@ -401,7 +401,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>7646.017492464823</v>
+        <v>5784.462396351928</v>
       </c>
     </row>
     <row r="12">
@@ -423,7 +423,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>40364.13333327451</v>
+        <v>27950.605714226906</v>
       </c>
     </row>
     <row r="14">
@@ -434,7 +434,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>40364.13333327451</v>
+        <v>27950.605714226906</v>
       </c>
     </row>
     <row r="15">
@@ -445,7 +445,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>30824.13333327452</v>
+        <v>18410.605714226906</v>
       </c>
     </row>
     <row r="16">
@@ -456,7 +456,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>30278.024385145814</v>
+        <v>18104.5475202269</v>
       </c>
     </row>
     <row r="17">
@@ -467,7 +467,7 @@
         <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>29742.545139274524</v>
+        <v>17329.01752022691</v>
       </c>
     </row>
     <row r="18">
@@ -489,7 +489,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>240.0507541286961</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
@@ -505,7 +505,7 @@
         <v>25</v>
       </c>
       <c r="C21" t="n">
-        <v>470818.74559523654</v>
+        <v>330828.0056866077</v>
       </c>
     </row>
     <row r="22">
@@ -516,7 +516,7 @@
         <v>25</v>
       </c>
       <c r="C22" t="n">
-        <v>470818.74559523654</v>
+        <v>330828.0056866077</v>
       </c>
     </row>
     <row r="23">
@@ -527,7 +527,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="n">
-        <v>456694.18322737946</v>
+        <v>320903.16551600944</v>
       </c>
     </row>
     <row r="24">
@@ -571,7 +571,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>395836.9281527564</v>
+        <v>274101.80752742314</v>
       </c>
     </row>
     <row r="28">
@@ -582,7 +582,7 @@
         <v>25</v>
       </c>
       <c r="C28" t="n">
-        <v>395836.9281527564</v>
+        <v>274101.80752742314</v>
       </c>
     </row>
     <row r="29">
@@ -593,7 +593,7 @@
         <v>25</v>
       </c>
       <c r="C29" t="n">
-        <v>302281.4871527564</v>
+        <v>180546.3665274232</v>
       </c>
     </row>
     <row r="30">
@@ -604,7 +604,7 @@
         <v>25</v>
       </c>
       <c r="C30" t="n">
-        <v>296925.98783659015</v>
+        <v>177544.96093923307</v>
       </c>
     </row>
     <row r="31">
@@ -615,7 +615,7 @@
         <v>25</v>
       </c>
       <c r="C31" t="n">
-        <v>291674.73029006645</v>
+        <v>169939.6096647332</v>
       </c>
     </row>
     <row r="32">
@@ -637,7 +637,7 @@
         <v>25</v>
       </c>
       <c r="C33" t="n">
-        <v>2354.0937279761765</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -725,10 +725,10 @@
         <v>43</v>
       </c>
       <c r="C7" t="n">
-        <v>4368.0</v>
+        <v>3909.0</v>
       </c>
       <c r="D7" t="n">
-        <v>12.868217054263592</v>
+        <v>1.00775193798452</v>
       </c>
     </row>
     <row r="8">
@@ -739,10 +739,10 @@
         <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>4573.0</v>
+        <v>3833.0</v>
       </c>
       <c r="D8" t="n">
-        <v>18.16537467700261</v>
+        <v>-0.9560723514211653</v>
       </c>
     </row>
     <row r="9">
@@ -753,10 +753,10 @@
         <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>4692.0</v>
+        <v>3356.0</v>
       </c>
       <c r="D9" t="n">
-        <v>21.240310077519407</v>
+        <v>-13.281653746770006</v>
       </c>
     </row>
     <row r="10">
@@ -795,10 +795,10 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>4935.166666666666</v>
+        <v>4512.666666666666</v>
       </c>
       <c r="D12" t="n">
-        <v>27.52368647717487</v>
+        <v>16.606373815676168</v>
       </c>
     </row>
   </sheetData>
@@ -883,10 +883,10 @@
         <v>43</v>
       </c>
       <c r="C7" t="n">
-        <v>3621.0</v>
+        <v>3021.0</v>
       </c>
       <c r="D7" t="n">
-        <v>40.348837209302374</v>
+        <v>17.093023255813993</v>
       </c>
     </row>
     <row r="8">
@@ -967,10 +967,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>2716.4285714285716</v>
+        <v>2630.7142857142853</v>
       </c>
       <c r="D13" t="n">
-        <v>5.287929125138451</v>
+        <v>1.965669988925823</v>
       </c>
     </row>
   </sheetData>
@@ -1069,10 +1069,10 @@
         <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>180.0</v>
+        <v>177.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-53.488372093023244</v>
+        <v>-54.26356589147286</v>
       </c>
     </row>
     <row r="9">
@@ -1083,10 +1083,10 @@
         <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>231.0</v>
+        <v>185.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-40.31007751937983</v>
+        <v>-52.19638242894055</v>
       </c>
     </row>
     <row r="10">
@@ -1097,10 +1097,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>243.0</v>
+        <v>226.66666666666663</v>
       </c>
       <c r="D10" t="n">
-        <v>-37.209302325581376</v>
+        <v>-41.42980189491815</v>
       </c>
     </row>
   </sheetData>
@@ -1470,7 +1470,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>11747.999999999996</v>
+        <v>3507.999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -1481,7 +1481,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>16176.995999999992</v>
+        <v>4830.515999999998</v>
       </c>
     </row>
     <row r="4">
@@ -1512,7 +1512,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>5874.0</v>
+        <v>1754.0</v>
       </c>
     </row>
     <row r="9">
@@ -1523,7 +1523,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>8088.497999999997</v>
+        <v>2415.257999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1544,7 +1544,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>5874.0</v>
+        <v>1754.0</v>
       </c>
     </row>
     <row r="13">
@@ -1555,7 +1555,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>8088.497999999997</v>
+        <v>2415.257999999999</v>
       </c>
     </row>
     <row r="14">
@@ -1623,10 +1623,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>1417.0</v>
+        <v>1053.0</v>
       </c>
       <c r="D5" t="n">
-        <v>37.306201550387655</v>
+        <v>2.0348837209302775</v>
       </c>
     </row>
     <row r="6">
@@ -1637,10 +1637,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>1920.0</v>
+        <v>1349.0</v>
       </c>
       <c r="D6" t="n">
-        <v>86.04651162790705</v>
+        <v>30.71705426356595</v>
       </c>
     </row>
     <row r="7">
@@ -1651,10 +1651,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>2178.0</v>
+        <v>1521.0</v>
       </c>
       <c r="D7" t="n">
-        <v>111.04651162790707</v>
+        <v>47.38372093023262</v>
       </c>
     </row>
     <row r="8">
@@ -1665,10 +1665,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>1945.0</v>
+        <v>1367.0</v>
       </c>
       <c r="D8" t="n">
-        <v>88.4689922480621</v>
+        <v>32.46124031007758</v>
       </c>
     </row>
     <row r="9">
@@ -1679,10 +1679,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>1865.0</v>
+        <v>1322.5</v>
       </c>
       <c r="D9" t="n">
-        <v>80.71705426356593</v>
+        <v>28.149224806201573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More tests A320, CS300, AGILE_NTP, DASH8
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/AGILE-NTP/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/AGILE-NTP/WEIGHTS/Weights.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="70">
   <si>
     <t>Description</t>
   </si>
@@ -64,6 +64,9 @@
     <t>Maximum Passengers Mass</t>
   </si>
   <si>
+    <t>Actual Passengers Mass</t>
+  </si>
+  <si>
     <t>Maximum Fuel Mass</t>
   </si>
   <si>
@@ -91,6 +94,9 @@
     <t>Operating Item Mass</t>
   </si>
   <si>
+    <t>Furnishings and Equipments Mass</t>
+  </si>
+  <si>
     <t>Trapped Fuel Oil Mass</t>
   </si>
   <si>
@@ -109,6 +115,9 @@
     <t>Maximum Passengers Weight</t>
   </si>
   <si>
+    <t>Actual Passengers Weight</t>
+  </si>
+  <si>
     <t>Fuel Weight</t>
   </si>
   <si>
@@ -131,6 +140,9 @@
   </si>
   <si>
     <t>Operating Item Weight</t>
+  </si>
+  <si>
+    <t>Furnishings and Equipments Weight</t>
   </si>
   <si>
     <t>Trapped Fuel Oil Weight</t>
@@ -346,7 +358,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>33735.068110578824</v>
+        <v>36242.802861219454</v>
       </c>
     </row>
     <row r="7">
@@ -357,7 +369,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>33735.068110578824</v>
+        <v>36242.802861219454</v>
       </c>
     </row>
     <row r="8">
@@ -368,7 +380,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>32723.01606726146</v>
+        <v>35155.518775382865</v>
       </c>
     </row>
     <row r="9">
@@ -390,7 +402,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>8740.769378449582</v>
+        <v>9540.0</v>
       </c>
     </row>
     <row r="11">
@@ -401,7 +413,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>5784.462396351928</v>
+        <v>8740.769378449582</v>
       </c>
     </row>
     <row r="12">
@@ -412,7 +424,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>306.05819399999996</v>
+        <v>6214.4570036714385</v>
       </c>
     </row>
     <row r="13">
@@ -423,7 +435,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>27950.605714226906</v>
+        <v>306.05819399999996</v>
       </c>
     </row>
     <row r="14">
@@ -434,7 +446,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>27950.605714226906</v>
+        <v>30028.345857548018</v>
       </c>
     </row>
     <row r="15">
@@ -445,7 +457,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>18410.605714226906</v>
+        <v>30028.345857548018</v>
       </c>
     </row>
     <row r="16">
@@ -456,7 +468,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>18104.5475202269</v>
+        <v>20488.34585754802</v>
       </c>
     </row>
     <row r="17">
@@ -467,7 +479,7 @@
         <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>17329.01752022691</v>
+        <v>20182.287663548017</v>
       </c>
     </row>
     <row r="18">
@@ -478,7 +490,7 @@
         <v>8</v>
       </c>
       <c r="C18" t="n">
-        <v>775.53</v>
+        <v>19406.757663548025</v>
       </c>
     </row>
     <row r="19">
@@ -489,45 +501,45 @@
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0</v>
+        <v>775.53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1886.7758576068286</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C21" t="n">
-        <v>330828.0056866077</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="n">
-        <v>330828.0056866077</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
       <c r="C23" t="n">
-        <v>320903.16551600944</v>
+        <v>355420.48267897766</v>
       </c>
     </row>
     <row r="24">
@@ -535,10 +547,10 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C24" t="n">
-        <v>93555.44099999996</v>
+        <v>355420.48267897766</v>
       </c>
     </row>
     <row r="25">
@@ -546,10 +558,10 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C25" t="n">
-        <v>85717.66602517257</v>
+        <v>344757.8681986083</v>
       </c>
     </row>
     <row r="26">
@@ -557,10 +569,10 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C26" t="n">
-        <v>3001.4055881900995</v>
+        <v>93555.44099999996</v>
       </c>
     </row>
     <row r="27">
@@ -568,10 +580,10 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C27" t="n">
-        <v>274101.80752742314</v>
+        <v>93555.44099999996</v>
       </c>
     </row>
     <row r="28">
@@ -579,10 +591,10 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>274101.80752742314</v>
+        <v>85717.66602517257</v>
       </c>
     </row>
     <row r="29">
@@ -590,10 +602,10 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C29" t="n">
-        <v>180546.3665274232</v>
+        <v>3001.4055881900995</v>
       </c>
     </row>
     <row r="30">
@@ -601,10 +613,10 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C30" t="n">
-        <v>177544.96093923307</v>
+        <v>294477.47790392314</v>
       </c>
     </row>
     <row r="31">
@@ -612,10 +624,10 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C31" t="n">
-        <v>169939.6096647332</v>
+        <v>294477.47790392314</v>
       </c>
     </row>
     <row r="32">
@@ -623,10 +635,10 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C32" t="n">
-        <v>7605.351274499997</v>
+        <v>200922.03690392326</v>
       </c>
     </row>
     <row r="33">
@@ -634,9 +646,53 @@
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C33" t="n">
+        <v>197920.63131573307</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="n">
+        <v>190315.2800412332</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="n">
+        <v>7605.351274499997</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="n">
+        <v>18502.950464</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -668,12 +724,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -684,7 +740,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -700,15 +756,15 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C6" t="n">
         <v>5962.0</v>
@@ -719,52 +775,52 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C7" t="n">
-        <v>3909.0</v>
+        <v>3998.0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.00775193798452</v>
+        <v>3.307493540051704</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C8" t="n">
-        <v>3833.0</v>
+        <v>3973.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.9560723514211653</v>
+        <v>2.66149870801036</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9" t="n">
-        <v>3356.0</v>
+        <v>3592.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-13.281653746770006</v>
+        <v>-7.183462532299719</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C10" t="n">
         <v>4408.0</v>
@@ -775,10 +831,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C11" t="n">
         <v>5608.0</v>
@@ -789,16 +845,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>4512.666666666666</v>
+        <v>4590.166666666666</v>
       </c>
       <c r="D12" t="n">
-        <v>16.606373815676168</v>
+        <v>18.608957795004333</v>
       </c>
     </row>
   </sheetData>
@@ -829,12 +885,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -845,18 +901,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.85</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -872,29 +928,29 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C7" t="n">
-        <v>3021.0</v>
+        <v>3124.0</v>
       </c>
       <c r="D7" t="n">
-        <v>17.093023255813993</v>
+        <v>21.0852713178295</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C8" t="n">
         <v>2486.0</v>
@@ -905,10 +961,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9" t="n">
         <v>2712.0</v>
@@ -919,10 +975,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C10" t="n">
         <v>3524.0</v>
@@ -933,10 +989,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C11" t="n">
         <v>3698.0</v>
@@ -947,10 +1003,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C12" t="n">
         <v>2974.0</v>
@@ -961,16 +1017,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>2630.7142857142853</v>
+        <v>2645.4285714285716</v>
       </c>
       <c r="D13" t="n">
-        <v>1.965669988925823</v>
+        <v>2.5359911406423263</v>
       </c>
     </row>
   </sheetData>
@@ -1001,12 +1057,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1017,7 +1073,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1028,7 +1084,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1044,15 +1100,15 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C7" t="n">
         <v>318.0</v>
@@ -1063,44 +1119,44 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C8" t="n">
-        <v>177.0</v>
+        <v>178.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-54.26356589147286</v>
+        <v>-54.005167958656315</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9" t="n">
-        <v>185.0</v>
+        <v>193.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-52.19638242894055</v>
+        <v>-50.129198966408254</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>226.66666666666663</v>
+        <v>229.66666666666663</v>
       </c>
       <c r="D10" t="n">
-        <v>-41.42980189491815</v>
+        <v>-40.654608096468536</v>
       </c>
     </row>
   </sheetData>
@@ -1131,12 +1187,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1147,7 +1203,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1158,7 +1214,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1174,15 +1230,15 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C7" t="n">
         <v>398.0</v>
@@ -1193,10 +1249,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C8" t="n">
         <v>277.0</v>
@@ -1207,7 +1263,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -1247,12 +1303,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1263,7 +1319,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1282,7 +1338,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
@@ -1292,12 +1348,12 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1306,10 +1362,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9" t="n">
         <v>84.0</v>
@@ -1320,10 +1376,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C10" t="n">
         <v>501.0</v>
@@ -1334,10 +1390,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C11" t="n">
         <v>309.0</v>
@@ -1348,7 +1404,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1364,12 +1420,12 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1378,10 +1434,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C16" t="n">
         <v>84.0</v>
@@ -1392,10 +1448,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C17" t="n">
         <v>501.0</v>
@@ -1406,10 +1462,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C18" t="n">
         <v>309.0</v>
@@ -1420,7 +1476,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1464,7 +1520,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1475,7 +1531,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1491,7 +1547,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
@@ -1501,12 +1557,12 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1517,7 +1573,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -1533,12 +1589,12 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1549,7 +1605,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -1591,12 +1647,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1612,77 +1668,77 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>1053.0</v>
+        <v>1119.0</v>
       </c>
       <c r="D5" t="n">
-        <v>2.0348837209302775</v>
+        <v>8.430232558139583</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>1349.0</v>
+        <v>1450.0</v>
       </c>
       <c r="D6" t="n">
-        <v>30.71705426356595</v>
+        <v>40.50387596899231</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>1521.0</v>
+        <v>1635.0</v>
       </c>
       <c r="D7" t="n">
-        <v>47.38372093023262</v>
+        <v>58.4302325581396</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>1367.0</v>
+        <v>1469.0</v>
       </c>
       <c r="D8" t="n">
-        <v>32.46124031007758</v>
+        <v>42.34496124031014</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>1322.5</v>
+        <v>1418.25</v>
       </c>
       <c r="D9" t="n">
-        <v>28.149224806201573</v>
+        <v>37.42732558139538</v>
       </c>
     </row>
   </sheetData>
@@ -1713,12 +1769,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1734,12 +1790,12 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -1753,7 +1809,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>

</xml_diff>